<commit_message>
add origin and location
</commit_message>
<xml_diff>
--- a/Hedges.xlsx
+++ b/Hedges.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88747f93bb6c7eaf/Documents/Postdoc UBC/Interactions paper/meta-analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88747f93bb6c7eaf/Documents/Postdoc UBC/Interactions paper/meta-analysis/interactions_salmonids/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2793" documentId="13_ncr:1_{3BF83E3E-61C9-45E5-BF17-F43AA12D13D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CC0FB23-9C2E-40BC-AB04-E9CA9BF0DF77}"/>
+  <xr:revisionPtr revIDLastSave="2867" documentId="13_ncr:1_{3BF83E3E-61C9-45E5-BF17-F43AA12D13D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82E58D35-53C2-4B69-9CCE-761F334ABD8A}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="11136" xr2:uid="{22809DD5-28F5-466E-A34A-A41D36053B95}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="412">
   <si>
     <t>Description</t>
   </si>
@@ -2245,9 +2245,6 @@
     <t>Farm</t>
   </si>
   <si>
-    <t>Britanny, FR</t>
-  </si>
-  <si>
     <t>River</t>
   </si>
   <si>
@@ -2279,6 +2276,36 @@
   </si>
   <si>
     <t>Haíɫzaqv Nation, CA</t>
+  </si>
+  <si>
+    <t>Oregon. USA</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>British Columbia, CA</t>
+  </si>
+  <si>
+    <t>Montana, USA</t>
+  </si>
+  <si>
+    <t>Herbert and Shurben, 1964</t>
+  </si>
+  <si>
+    <t>Amonia</t>
+  </si>
+  <si>
+    <t>Herbert, D.W.M. and Surben, D.S. (1964), The toxicity to fish of mixtures of poisons. Annals of Applied Biology, 53: 33-41. https://doi.org/10.1111/j.1744-7348.1964.tb03778.x</t>
+  </si>
+  <si>
+    <t>Turkey</t>
   </si>
 </sst>
 </file>
@@ -2383,7 +2410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2534,6 +2561,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2549,10 +2579,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2852,11 +2878,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1C84BB-F2CC-42C6-A1BF-21ED272783EE}">
-  <dimension ref="A1:X93"/>
+  <dimension ref="A1:X94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5376,7 +5402,7 @@
         <v>390</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>19</v>
@@ -5441,7 +5467,7 @@
         <v>134</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>377</v>
@@ -5518,7 +5544,7 @@
         <v>390</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>19</v>
@@ -5592,7 +5618,7 @@
         <v>382</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>19</v>
@@ -5651,7 +5677,7 @@
         <v>373</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>19</v>
@@ -5781,7 +5807,7 @@
         <v>390</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>19</v>
@@ -5985,7 +6011,7 @@
         <v>373</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>19</v>
@@ -6032,7 +6058,7 @@
         <v>1992</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>7</v>
@@ -6103,7 +6129,7 @@
         <v>390</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>19</v>
@@ -6162,7 +6188,7 @@
         <v>390</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G52" s="21" t="s">
         <v>19</v>
@@ -6475,7 +6501,7 @@
         <v>373</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>19</v>
@@ -6537,7 +6563,7 @@
         <v>373</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G58" s="20" t="s">
         <v>19</v>
@@ -6648,7 +6674,7 @@
         <v>382</v>
       </c>
       <c r="F60" s="30" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G60" s="30" t="s">
         <v>19</v>
@@ -6825,10 +6851,10 @@
         <v>172</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G63" s="14" t="s">
         <v>16</v>
@@ -6877,7 +6903,7 @@
         <v>123</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F64" s="14" t="s">
         <v>368</v>
@@ -7026,8 +7052,12 @@
       <c r="D67" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
+      <c r="E67" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>402</v>
+      </c>
       <c r="G67" s="14" t="s">
         <v>19</v>
       </c>
@@ -7065,8 +7095,12 @@
       <c r="D68" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
+      <c r="E68" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>375</v>
+      </c>
       <c r="G68" s="14" t="s">
         <v>19</v>
       </c>
@@ -7104,8 +7138,12 @@
       <c r="D69" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
+      <c r="E69" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>394</v>
+      </c>
       <c r="G69" s="14" t="s">
         <v>16</v>
       </c>
@@ -7143,8 +7181,12 @@
       <c r="D70" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
+      <c r="E70" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>393</v>
+      </c>
       <c r="G70" s="14" t="s">
         <v>19</v>
       </c>
@@ -7185,8 +7227,12 @@
       <c r="D71" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
+      <c r="E71" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>403</v>
+      </c>
       <c r="G71" s="14" t="s">
         <v>19</v>
       </c>
@@ -7224,8 +7270,12 @@
       <c r="D72" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
+      <c r="E72" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>404</v>
+      </c>
       <c r="G72" s="14" t="s">
         <v>16</v>
       </c>
@@ -7263,8 +7313,12 @@
       <c r="D73" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
+      <c r="E73" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>402</v>
+      </c>
       <c r="G73" s="14" t="s">
         <v>293</v>
       </c>
@@ -7302,8 +7356,12 @@
       <c r="D74" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
+      <c r="E74" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F74" s="14" t="s">
+        <v>377</v>
+      </c>
       <c r="G74" s="14" t="s">
         <v>19</v>
       </c>
@@ -7347,8 +7405,12 @@
       <c r="D75" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
+      <c r="E75" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>368</v>
+      </c>
       <c r="G75" s="14" t="s">
         <v>19</v>
       </c>
@@ -7392,8 +7454,12 @@
       <c r="D76" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
+      <c r="E76" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>405</v>
+      </c>
       <c r="G76" s="14" t="s">
         <v>19</v>
       </c>
@@ -7431,8 +7497,12 @@
       <c r="D77" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
+      <c r="E77" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F77" s="14" t="s">
+        <v>383</v>
+      </c>
       <c r="G77" s="14" t="s">
         <v>19</v>
       </c>
@@ -7470,8 +7540,12 @@
       <c r="D78" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
+      <c r="E78" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F78" s="14" t="s">
+        <v>406</v>
+      </c>
       <c r="G78" s="14" t="s">
         <v>19</v>
       </c>
@@ -7509,8 +7583,12 @@
       <c r="D79" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
+      <c r="E79" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F79" s="14" t="s">
+        <v>123</v>
+      </c>
       <c r="G79" s="14" t="s">
         <v>16</v>
       </c>
@@ -7548,8 +7626,12 @@
       <c r="D80" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
+      <c r="E80" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F80" s="14" t="s">
+        <v>123</v>
+      </c>
       <c r="G80" s="14" t="s">
         <v>16</v>
       </c>
@@ -7587,8 +7669,12 @@
       <c r="D81" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
+      <c r="E81" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="F81" s="14" t="s">
+        <v>123</v>
+      </c>
       <c r="G81" s="14" t="s">
         <v>19</v>
       </c>
@@ -7626,8 +7712,12 @@
       <c r="D82" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
+      <c r="E82" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>123</v>
+      </c>
       <c r="G82" s="14" t="s">
         <v>19</v>
       </c>
@@ -7665,8 +7755,12 @@
       <c r="D83" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
+      <c r="E83" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>407</v>
+      </c>
       <c r="G83" s="14" t="s">
         <v>19</v>
       </c>
@@ -7704,8 +7798,12 @@
       <c r="D84" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
+      <c r="E84" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>123</v>
+      </c>
       <c r="G84" s="14" t="s">
         <v>19</v>
       </c>
@@ -7743,8 +7841,12 @@
       <c r="D85" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
+      <c r="E85" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F85" s="14" t="s">
+        <v>402</v>
+      </c>
       <c r="G85" s="14" t="s">
         <v>19</v>
       </c>
@@ -7782,8 +7884,12 @@
       <c r="D86" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
+      <c r="E86" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>383</v>
+      </c>
       <c r="G86" s="14" t="s">
         <v>19</v>
       </c>
@@ -7821,8 +7927,12 @@
       <c r="D87" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E87" s="25"/>
-      <c r="F87" s="25"/>
+      <c r="E87" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="F87" s="25" t="s">
+        <v>411</v>
+      </c>
       <c r="G87" s="25" t="s">
         <v>19</v>
       </c>
@@ -7860,8 +7970,12 @@
       <c r="D88" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E88" s="25"/>
-      <c r="F88" s="25"/>
+      <c r="E88" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="F88" s="25" t="s">
+        <v>411</v>
+      </c>
       <c r="G88" s="25" t="s">
         <v>19</v>
       </c>
@@ -7899,8 +8013,12 @@
       <c r="D89" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="E89" s="25"/>
-      <c r="F89" s="25"/>
+      <c r="E89" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="F89" s="25" t="s">
+        <v>381</v>
+      </c>
       <c r="G89" s="25" t="s">
         <v>19</v>
       </c>
@@ -7938,8 +8056,12 @@
       <c r="D90" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
+      <c r="E90" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="F90" s="25" t="s">
+        <v>381</v>
+      </c>
       <c r="G90" s="25" t="s">
         <v>19</v>
       </c>
@@ -7977,8 +8099,12 @@
       <c r="D91" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
+      <c r="E91" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="F91" s="25" t="s">
+        <v>381</v>
+      </c>
       <c r="G91" s="25" t="s">
         <v>19</v>
       </c>
@@ -8016,8 +8142,12 @@
       <c r="D92" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
+      <c r="E92" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="F92" s="25" t="s">
+        <v>381</v>
+      </c>
       <c r="G92" s="25" t="s">
         <v>19</v>
       </c>
@@ -8064,8 +8194,12 @@
       <c r="D93" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="E93" s="25"/>
-      <c r="F93" s="25"/>
+      <c r="E93" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="F93" s="25" t="s">
+        <v>381</v>
+      </c>
       <c r="G93" s="25" t="s">
         <v>19</v>
       </c>
@@ -8097,6 +8231,41 @@
       </c>
       <c r="X93" s="38" t="s">
         <v>247</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="1">
+        <v>1964</v>
+      </c>
+      <c r="B94" s="58" t="s">
+        <v>408</v>
+      </c>
+      <c r="C94" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="D94" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="E94" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="F94" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="G94" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="H94" s="58" t="s">
+        <v>409</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="X94" s="8" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>